<commit_message>
Update GL code Nov24
</commit_message>
<xml_diff>
--- a/Balance Sheet - Dictionary.xlsx
+++ b/Balance Sheet - Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git Repository\EXIM-Bank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848B8942-16E9-441C-9D32-001227E77558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1100B6C1-3917-4C67-95B8-B6E49C4E1E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13545" yWindow="4635" windowWidth="14610" windowHeight="9525" firstSheet="19" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cash Bank" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4029" uniqueCount="1182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4032" uniqueCount="1183">
   <si>
     <t>GL Description</t>
   </si>
@@ -3604,6 +3604,9 @@
   </si>
   <si>
     <t>BNM All Economic Sectors (AES) Program</t>
+  </si>
+  <si>
+    <t>Profit Penalty Loan Debtors</t>
   </si>
 </sst>
 </file>
@@ -17381,8 +17384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7AE4F43-2689-4F67-A74F-D6C613839384}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18587,8 +18590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DA38C58-27F6-4751-84AA-B8BFF990A065}">
   <dimension ref="A1:E83"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19029,6 +19032,18 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B28">
+        <v>1134002</v>
+      </c>
+      <c r="C28" t="s">
+        <v>272</v>
+      </c>
+      <c r="D28" t="s">
+        <v>268</v>
+      </c>
       <c r="E28" t="s">
         <v>265</v>
       </c>

</xml_diff>